<commit_message>
update extract multiple sheets and display
</commit_message>
<xml_diff>
--- a/src/jw/app/excel/mytest.xlsx
+++ b/src/jw/app/excel/mytest.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\myGoPro\src\jw\app\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4545D0-0456-4200-9D5B-074101F2B940}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF1F66E-F32E-482A-AF68-EAFFC844CCD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="部门信息" sheetId="1" r:id="rId1"/>
-    <sheet name="sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="运输部" sheetId="1" r:id="rId1"/>
+    <sheet name="财务部" sheetId="2" r:id="rId2"/>
+    <sheet name="会计部" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
   <si>
     <t>姓名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,6 +72,46 @@
   <si>
     <t>运输部</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>财务部</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>会计部</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>李1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>李2</t>
+  </si>
+  <si>
+    <t>李3</t>
+  </si>
+  <si>
+    <t>童3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>童4</t>
+  </si>
+  <si>
+    <t>童5</t>
+  </si>
+  <si>
+    <t>童6</t>
+  </si>
+  <si>
+    <t>童7</t>
+  </si>
+  <si>
+    <t>童8</t>
+  </si>
+  <si>
+    <t>童9</t>
   </si>
 </sst>
 </file>
@@ -400,7 +440,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -555,12 +595,130 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BC16ECC-66F0-4FBC-B168-5B19C87F40E9}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1">
+        <v>43809</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1">
+        <v>43810</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1">
+        <v>43811</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1">
+        <v>43813</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1">
+        <v>43814</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1">
+        <v>43815</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -569,14 +727,74 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{962D067E-FEA7-4FA4-A4D5-9071BC725914}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1">
+        <v>43809</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1">
+        <v>43810</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1">
+        <v>43811</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>